<commit_message>
Se modifica el nombre de las columnas
</commit_message>
<xml_diff>
--- a/Dataset/AgriculturaIndia.xlsx
+++ b/Dataset/AgriculturaIndia.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{725DE05E-6CE2-4BFB-9AA6-D0245BDFCF2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3098C392-F30D-49EC-8A88-28EEFCC05EB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="5040" yWindow="3084" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datafile" sheetId="1" r:id="rId1"/>
@@ -28,15 +28,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>Cost of Cultivation (`/Hectare) A2+FL</t>
-  </si>
-  <si>
-    <t>Cost of Cultivation (`/Hectare) C2</t>
-  </si>
-  <si>
-    <t>Cost of Production (`/Quintal) C2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yield (Quintal/ Hectare) </t>
   </si>
   <si>
@@ -107,12 +98,21 @@
   </si>
   <si>
     <t>WHEAT</t>
+  </si>
+  <si>
+    <t>Cost of Cultivation (/ Hectare) A2+FL</t>
+  </si>
+  <si>
+    <t>Cost of Cultivation (/ Hectare) C2</t>
+  </si>
+  <si>
+    <t>Cost of Production (/ Quintal) C2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -946,11 +946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,24 +971,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>9794.0499999999993</v>
@@ -1005,10 +1005,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>10593.15</v>
@@ -1025,10 +1025,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4">
         <v>13468.82</v>
@@ -1045,10 +1045,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>17051.66</v>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>17130.55</v>
@@ -1085,10 +1085,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>23711.439999999999</v>
@@ -1105,10 +1105,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>29047.1</v>
@@ -1125,10 +1125,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>29140.77</v>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>29616.09</v>
@@ -1165,10 +1165,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>29918.97</v>
@@ -1185,10 +1185,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>8552.69</v>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>9803.89</v>
@@ -1225,10 +1225,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>12833.04</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>12985.95</v>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>14421.98</v>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>13647.1</v>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>21229.01</v>
@@ -1325,10 +1325,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>22507.86</v>
@@ -1345,10 +1345,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>22951.279999999999</v>
@@ -1365,10 +1365,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>26078.66</v>
@@ -1385,10 +1385,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>13513.92</v>
@@ -1405,10 +1405,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>13792.85</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>14421.46</v>
@@ -1445,10 +1445,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>15635.43</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C26">
         <v>25687.09</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27">
         <v>5483.54</v>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C28">
         <v>6204.23</v>
@@ -1525,10 +1525,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>6440.64</v>
@@ -1545,10 +1545,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C30">
         <v>6684.18</v>
@@ -1565,10 +1565,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C31">
         <v>10780.76</v>
@@ -1585,10 +1585,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>17022</v>
@@ -1605,10 +1605,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C33">
         <v>17478.05</v>
@@ -1625,10 +1625,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>24731.06</v>
@@ -1645,10 +1645,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C35">
         <v>25154.75</v>
@@ -1665,10 +1665,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C36">
         <v>29664.84</v>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C37">
         <v>8686.43</v>
@@ -1705,10 +1705,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C38">
         <v>11385.7</v>
@@ -1725,10 +1725,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>12774.41</v>
@@ -1745,10 +1745,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>13740.64</v>
@@ -1765,10 +1765,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C41">
         <v>14715.27</v>
@@ -1785,10 +1785,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>24538.32</v>
@@ -1805,10 +1805,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>55655.44</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>56621.16</v>
@@ -1845,10 +1845,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>57673.599999999999</v>
@@ -1865,10 +1865,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C46">
         <v>66335.06</v>
@@ -1885,10 +1885,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C47">
         <v>12464.4</v>
@@ -1905,10 +1905,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C48">
         <v>17945.580000000002</v>
@@ -1925,10 +1925,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>18979.38</v>
@@ -1945,10 +1945,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C50">
         <v>19119.080000000002</v>

</xml_diff>

<commit_message>
Se modifica clase Agricultura
</commit_message>
<xml_diff>
--- a/Dataset/AgriculturaIndia.xlsx
+++ b/Dataset/AgriculturaIndia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3098C392-F30D-49EC-8A88-28EEFCC05EB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF442AB-BAC8-4BCD-924C-27246818D508}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="3084" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datafile" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="29">
   <si>
     <t>Crop</t>
   </si>
@@ -947,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,379 +1085,379 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>23711.439999999999</v>
+        <v>12001.21</v>
       </c>
       <c r="D7">
-        <v>33116.82</v>
+        <v>23293.24</v>
       </c>
       <c r="E7">
-        <v>2539.4699999999998</v>
+        <v>1700.8</v>
       </c>
       <c r="F7">
-        <v>12.69</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>29047.1</v>
+        <v>11733.15</v>
       </c>
       <c r="D8">
-        <v>50828.83</v>
+        <v>21722.46</v>
       </c>
       <c r="E8">
-        <v>2003.76</v>
+        <v>2528.6799999999998</v>
       </c>
       <c r="F8">
-        <v>24.39</v>
+        <v>9.0500000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>29140.77</v>
+        <v>12233.04</v>
       </c>
       <c r="D9">
-        <v>44756.72</v>
+        <v>18618.43</v>
       </c>
       <c r="E9">
-        <v>2509.9899999999998</v>
+        <v>1982.78</v>
       </c>
       <c r="F9">
-        <v>17.829999999999998</v>
+        <v>10.91</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>29616.09</v>
+        <v>13722.85</v>
       </c>
       <c r="D10">
-        <v>42070.44</v>
+        <v>16857.7</v>
       </c>
       <c r="E10">
-        <v>2179.2600000000002</v>
+        <v>1403.43</v>
       </c>
       <c r="F10">
-        <v>19.05</v>
+        <v>8.9499999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>29918.97</v>
+        <v>15421.46</v>
       </c>
       <c r="D11">
-        <v>44018.18</v>
+        <v>18228.88</v>
       </c>
       <c r="E11">
-        <v>2127.35</v>
+        <v>1958.77</v>
       </c>
       <c r="F11">
-        <v>19.899999999999999</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>8552.69</v>
+        <v>23711.439999999999</v>
       </c>
       <c r="D12">
-        <v>12610.85</v>
+        <v>33116.82</v>
       </c>
       <c r="E12">
-        <v>1691.66</v>
+        <v>2539.4699999999998</v>
       </c>
       <c r="F12">
-        <v>6.83</v>
+        <v>12.69</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>9803.89</v>
+        <v>29047.1</v>
       </c>
       <c r="D13">
-        <v>16873.169999999998</v>
+        <v>50828.83</v>
       </c>
       <c r="E13">
-        <v>1551.94</v>
+        <v>2003.76</v>
       </c>
       <c r="F13">
-        <v>10.29</v>
+        <v>24.39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>12833.04</v>
+        <v>29140.77</v>
       </c>
       <c r="D14">
-        <v>21618.43</v>
+        <v>44756.72</v>
       </c>
       <c r="E14">
-        <v>1882.68</v>
+        <v>2509.9899999999998</v>
       </c>
       <c r="F14">
-        <v>10.93</v>
+        <v>17.829999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>12985.95</v>
+        <v>29616.09</v>
       </c>
       <c r="D15">
-        <v>18679.330000000002</v>
+        <v>42070.44</v>
       </c>
       <c r="E15">
-        <v>2277.6799999999998</v>
+        <v>2179.2600000000002</v>
       </c>
       <c r="F15">
-        <v>8.0500000000000007</v>
+        <v>19.05</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>14421.98</v>
+        <v>29918.97</v>
       </c>
       <c r="D16">
-        <v>26762.09</v>
+        <v>44018.18</v>
       </c>
       <c r="E16">
-        <v>1559.04</v>
+        <v>2127.35</v>
       </c>
       <c r="F16">
-        <v>16.690000000000001</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>13647.1</v>
+        <v>25635.43</v>
       </c>
       <c r="D17">
-        <v>17314.2</v>
+        <v>51045.11</v>
       </c>
       <c r="E17">
-        <v>3484.01</v>
+        <v>2367.36</v>
       </c>
       <c r="F17">
-        <v>4.71</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>21229.01</v>
+        <v>28229.01</v>
       </c>
       <c r="D18">
-        <v>30434.61</v>
+        <v>40431.61</v>
       </c>
       <c r="E18">
-        <v>2554.91</v>
+        <v>2514.5100000000002</v>
       </c>
       <c r="F18">
-        <v>11.97</v>
+        <v>21.98</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19">
-        <v>22507.86</v>
+        <v>8552.69</v>
       </c>
       <c r="D19">
-        <v>30393.66</v>
+        <v>12610.85</v>
       </c>
       <c r="E19">
-        <v>2358</v>
+        <v>1691.66</v>
       </c>
       <c r="F19">
-        <v>11.98</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C20">
-        <v>22951.279999999999</v>
+        <v>9803.89</v>
       </c>
       <c r="D20">
-        <v>30114.45</v>
+        <v>16873.169999999998</v>
       </c>
       <c r="E20">
-        <v>1918.92</v>
+        <v>1551.94</v>
       </c>
       <c r="F20">
-        <v>13.45</v>
+        <v>10.29</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>26078.66</v>
+        <v>12833.04</v>
       </c>
       <c r="D21">
-        <v>32683.46</v>
+        <v>21618.43</v>
       </c>
       <c r="E21">
-        <v>3207.35</v>
+        <v>1882.68</v>
       </c>
       <c r="F21">
-        <v>9.33</v>
+        <v>10.93</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>13513.92</v>
+        <v>12985.95</v>
       </c>
       <c r="D22">
-        <v>19857.7</v>
+        <v>18679.330000000002</v>
       </c>
       <c r="E22">
-        <v>404.43</v>
+        <v>2277.6799999999998</v>
       </c>
       <c r="F22">
-        <v>42.95</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>13792.85</v>
+        <v>14421.98</v>
       </c>
       <c r="D23">
-        <v>20671.54</v>
+        <v>26762.09</v>
       </c>
       <c r="E23">
-        <v>581.69000000000005</v>
+        <v>1559.04</v>
       </c>
       <c r="F23">
-        <v>31.1</v>
+        <v>16.690000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C24">
-        <v>14421.46</v>
+        <v>12130.55</v>
       </c>
       <c r="D24">
-        <v>19810.29</v>
+        <v>20570.259999999998</v>
       </c>
       <c r="E24">
-        <v>658.77</v>
+        <v>1875.8</v>
       </c>
       <c r="F24">
-        <v>23.56</v>
+        <v>9.02</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>15635.43</v>
+        <v>11814.76</v>
       </c>
       <c r="D25">
-        <v>21045.11</v>
+        <v>14172.45</v>
       </c>
       <c r="E25">
-        <v>1387.36</v>
+        <v>2201.2399999999998</v>
       </c>
       <c r="F25">
         <v>13.7</v>
@@ -1465,505 +1465,786 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26">
-        <v>25687.09</v>
+        <v>12974.31</v>
       </c>
       <c r="D26">
-        <v>37801.85</v>
+        <v>21560.3</v>
       </c>
       <c r="E26">
-        <v>840.58</v>
+        <v>1835.56</v>
       </c>
       <c r="F26">
-        <v>42.68</v>
+        <v>10.57</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>5483.54</v>
+        <v>13647.1</v>
       </c>
       <c r="D27">
-        <v>8266.98</v>
+        <v>17314.2</v>
       </c>
       <c r="E27">
-        <v>2614.14</v>
+        <v>3484.01</v>
       </c>
       <c r="F27">
-        <v>3.01</v>
+        <v>4.71</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>6204.23</v>
+        <v>21229.01</v>
       </c>
       <c r="D28">
-        <v>9165.59</v>
+        <v>30434.61</v>
       </c>
       <c r="E28">
-        <v>2068.67</v>
+        <v>2554.91</v>
       </c>
       <c r="F28">
-        <v>4.05</v>
+        <v>11.97</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>6440.64</v>
+        <v>22507.86</v>
       </c>
       <c r="D29">
-        <v>7868.64</v>
+        <v>30393.66</v>
       </c>
       <c r="E29">
-        <v>5777.48</v>
+        <v>2358</v>
       </c>
       <c r="F29">
-        <v>1.32</v>
+        <v>11.98</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30">
-        <v>6684.18</v>
+        <v>22951.279999999999</v>
       </c>
       <c r="D30">
-        <v>13209.32</v>
+        <v>30114.45</v>
       </c>
       <c r="E30">
-        <v>2228.9699999999998</v>
+        <v>1918.92</v>
       </c>
       <c r="F30">
-        <v>5.9</v>
+        <v>13.45</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>10780.76</v>
+        <v>21258.66</v>
       </c>
       <c r="D31">
-        <v>15371.45</v>
+        <v>31653.46</v>
       </c>
       <c r="E31">
-        <v>2261.2399999999998</v>
+        <v>2627.35</v>
       </c>
       <c r="F31">
-        <v>6.7</v>
+        <v>12.31</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C32">
-        <v>17022</v>
+        <v>26078.66</v>
       </c>
       <c r="D32">
-        <v>28144.5</v>
+        <v>32683.46</v>
       </c>
       <c r="E32">
-        <v>732.62</v>
+        <v>3207.35</v>
       </c>
       <c r="F32">
-        <v>36.61</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C33">
-        <v>17478.05</v>
+        <v>13513.92</v>
       </c>
       <c r="D33">
-        <v>25909.05</v>
+        <v>19857.7</v>
       </c>
       <c r="E33">
-        <v>715.04</v>
+        <v>404.43</v>
       </c>
       <c r="F33">
-        <v>32.42</v>
+        <v>42.95</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C34">
-        <v>24731.06</v>
+        <v>14421.46</v>
       </c>
       <c r="D34">
-        <v>33046.120000000003</v>
+        <v>19810.29</v>
       </c>
       <c r="E34">
-        <v>731.25</v>
+        <v>658.77</v>
       </c>
       <c r="F34">
-        <v>39.04</v>
+        <v>23.56</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>25154.75</v>
+        <v>15635.43</v>
       </c>
       <c r="D35">
-        <v>45291.24</v>
+        <v>21045.11</v>
       </c>
       <c r="E35">
-        <v>669.86</v>
+        <v>1387.36</v>
       </c>
       <c r="F35">
-        <v>67.41</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
       <c r="C36">
-        <v>29664.84</v>
+        <v>25687.09</v>
       </c>
       <c r="D36">
-        <v>46450.2</v>
+        <v>37801.85</v>
       </c>
       <c r="E36">
-        <v>789.9</v>
+        <v>840.58</v>
       </c>
       <c r="F36">
-        <v>56</v>
+        <v>42.68</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>8686.43</v>
+        <v>5483.54</v>
       </c>
       <c r="D37">
-        <v>17705.93</v>
+        <v>8266.98</v>
       </c>
       <c r="E37">
-        <v>1279.5999999999999</v>
+        <v>2614.14</v>
       </c>
       <c r="F37">
-        <v>12.94</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
       <c r="C38">
-        <v>11385.7</v>
+        <v>6204.23</v>
       </c>
       <c r="D38">
-        <v>19259.84</v>
+        <v>9165.59</v>
       </c>
       <c r="E38">
-        <v>1341.29</v>
+        <v>2068.67</v>
       </c>
       <c r="F38">
-        <v>13.54</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>12774.41</v>
+        <v>6440.64</v>
       </c>
       <c r="D39">
-        <v>22560.3</v>
+        <v>7868.64</v>
       </c>
       <c r="E39">
-        <v>1595.56</v>
+        <v>5777.48</v>
       </c>
       <c r="F39">
-        <v>13.57</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <v>13740.64</v>
+        <v>6684.18</v>
       </c>
       <c r="D40">
-        <v>19083.55</v>
+        <v>13209.32</v>
       </c>
       <c r="E40">
-        <v>1610.4</v>
+        <v>2228.9699999999998</v>
       </c>
       <c r="F40">
-        <v>11.61</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>14715.27</v>
+        <v>6552.69</v>
       </c>
       <c r="D41">
-        <v>27507.54</v>
+        <v>11610.85</v>
       </c>
       <c r="E41">
-        <v>1251.1199999999999</v>
+        <v>2691.66</v>
       </c>
       <c r="F41">
-        <v>19.940000000000001</v>
+        <v>4.83</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C42">
-        <v>24538.32</v>
+        <v>7303.89</v>
       </c>
       <c r="D42">
-        <v>45239.51</v>
+        <v>12573.17</v>
       </c>
       <c r="E42">
-        <v>93.64</v>
+        <v>4551.9399999999996</v>
       </c>
       <c r="F42">
-        <v>448.89</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>55655.44</v>
+        <v>10780.76</v>
       </c>
       <c r="D43">
-        <v>86765.77</v>
+        <v>15371.45</v>
       </c>
       <c r="E43">
-        <v>86.53</v>
+        <v>2261.2399999999998</v>
       </c>
       <c r="F43">
-        <v>986.21</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>56621.16</v>
+        <v>17022</v>
       </c>
       <c r="D44">
-        <v>91442.63</v>
+        <v>28144.5</v>
       </c>
       <c r="E44">
-        <v>119.72</v>
+        <v>732.62</v>
       </c>
       <c r="F44">
-        <v>757.92</v>
+        <v>36.61</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>57673.599999999999</v>
+        <v>13792.85</v>
       </c>
       <c r="D45">
-        <v>85801.95</v>
+        <v>20671.54</v>
       </c>
       <c r="E45">
-        <v>107.56</v>
+        <v>581.69000000000005</v>
       </c>
       <c r="F45">
-        <v>744.01</v>
+        <v>31.1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C46">
-        <v>66335.06</v>
+        <v>17478.05</v>
       </c>
       <c r="D46">
-        <v>89025.27</v>
+        <v>25909.05</v>
       </c>
       <c r="E46">
-        <v>85.79</v>
+        <v>715.04</v>
       </c>
       <c r="F46">
-        <v>1015.45</v>
+        <v>32.42</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C47">
-        <v>12464.4</v>
+        <v>24731.06</v>
       </c>
       <c r="D47">
-        <v>22489.75</v>
+        <v>33046.120000000003</v>
       </c>
       <c r="E47">
-        <v>810.25</v>
+        <v>731.25</v>
       </c>
       <c r="F47">
-        <v>23.59</v>
+        <v>39.04</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="C48">
-        <v>17945.580000000002</v>
+        <v>25154.75</v>
       </c>
       <c r="D48">
-        <v>35423.480000000003</v>
+        <v>45291.24</v>
       </c>
       <c r="E48">
-        <v>804.8</v>
+        <v>669.86</v>
       </c>
       <c r="F48">
-        <v>39.83</v>
+        <v>67.41</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C49">
-        <v>18979.38</v>
+        <v>29664.84</v>
       </c>
       <c r="D49">
-        <v>31902.74</v>
+        <v>46450.2</v>
       </c>
       <c r="E49">
-        <v>769.84</v>
+        <v>789.9</v>
       </c>
       <c r="F49">
-        <v>34.99</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>8686.43</v>
+      </c>
+      <c r="D50">
+        <v>17705.93</v>
+      </c>
+      <c r="E50">
+        <v>1279.5999999999999</v>
+      </c>
+      <c r="F50">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>11385.7</v>
+      </c>
+      <c r="D51">
+        <v>19259.84</v>
+      </c>
+      <c r="E51">
+        <v>1341.29</v>
+      </c>
+      <c r="F51">
+        <v>13.54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>12774.41</v>
+      </c>
+      <c r="D52">
+        <v>22560.3</v>
+      </c>
+      <c r="E52">
+        <v>1595.56</v>
+      </c>
+      <c r="F52">
+        <v>13.57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>13740.64</v>
+      </c>
+      <c r="D53">
+        <v>19083.55</v>
+      </c>
+      <c r="E53">
+        <v>1610.4</v>
+      </c>
+      <c r="F53">
+        <v>11.61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>14715.27</v>
+      </c>
+      <c r="D54">
+        <v>27507.54</v>
+      </c>
+      <c r="E54">
+        <v>1251.1199999999999</v>
+      </c>
+      <c r="F54">
+        <v>19.940000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>24538.32</v>
+      </c>
+      <c r="D55">
+        <v>45239.51</v>
+      </c>
+      <c r="E55">
+        <v>93.64</v>
+      </c>
+      <c r="F55">
+        <v>448.89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>31235.06</v>
+      </c>
+      <c r="D56">
+        <v>45135.27</v>
+      </c>
+      <c r="E56">
+        <v>95.79</v>
+      </c>
+      <c r="F56">
+        <v>885.45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>55655.44</v>
+      </c>
+      <c r="D57">
+        <v>86765.77</v>
+      </c>
+      <c r="E57">
+        <v>86.53</v>
+      </c>
+      <c r="F57">
+        <v>986.21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <v>56621.16</v>
+      </c>
+      <c r="D58">
+        <v>91442.63</v>
+      </c>
+      <c r="E58">
+        <v>119.72</v>
+      </c>
+      <c r="F58">
+        <v>757.92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>57673.599999999999</v>
+      </c>
+      <c r="D59">
+        <v>85801.95</v>
+      </c>
+      <c r="E59">
+        <v>107.56</v>
+      </c>
+      <c r="F59">
+        <v>744.01</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60">
+        <v>66335.06</v>
+      </c>
+      <c r="D60">
+        <v>89025.27</v>
+      </c>
+      <c r="E60">
+        <v>85.79</v>
+      </c>
+      <c r="F60">
+        <v>1015.45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>25</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61">
+        <v>12464.4</v>
+      </c>
+      <c r="D61">
+        <v>22489.75</v>
+      </c>
+      <c r="E61">
+        <v>810.25</v>
+      </c>
+      <c r="F61">
+        <v>23.59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <v>17945.580000000002</v>
+      </c>
+      <c r="D62">
+        <v>35423.480000000003</v>
+      </c>
+      <c r="E62">
+        <v>804.8</v>
+      </c>
+      <c r="F62">
+        <v>39.83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>18979.38</v>
+      </c>
+      <c r="D63">
+        <v>31902.74</v>
+      </c>
+      <c r="E63">
+        <v>769.84</v>
+      </c>
+      <c r="F63">
+        <v>34.99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" t="s">
         <v>13</v>
       </c>
-      <c r="C50">
+      <c r="C64">
         <v>19119.080000000002</v>
       </c>
-      <c r="D50">
+      <c r="D64">
         <v>29876.36</v>
       </c>
-      <c r="E50">
+      <c r="E64">
         <v>683.58</v>
       </c>
-      <c r="F50">
+      <c r="F64">
         <v>37.19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>